<commit_message>
Tried to squash commits after removing large files from tracking
</commit_message>
<xml_diff>
--- a/06_inputs/i01_mappings.xlsx
+++ b/06_inputs/i01_mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\apartment_shopping\06_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A348FBAD-C233-47E5-8CC3-216A6CE2DB1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FD3770-24EE-42C6-AC1F-509347C953D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{9A8069C6-F8B2-476C-84DD-BB1A0B4AE697}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{9A8069C6-F8B2-476C-84DD-BB1A0B4AE697}"/>
   </bookViews>
   <sheets>
     <sheet name="used_mappings" sheetId="1" r:id="rId1"/>
@@ -1984,10 +1984,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AE61A00-CA00-4DE7-A6D0-2016F1E0A263}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{4A9543A1-C6ED-40CC-A971-1204199618FF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B4">
-    <sortCondition ref="A1:A4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AE61A00-CA00-4DE7-A6D0-2016F1E0A263}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{4A9543A1-C6ED-40CC-A971-1204199618FF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B3">
+    <sortCondition ref="A1:A3"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="4" xr3:uid="{BA6E9F97-2E8A-4D9D-81F3-089A7127BF02}" name="Hemnet_name"/>
@@ -1998,8 +1998,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F1800A77-6274-4EBD-A91A-8D8CA5AD2BBD}" name="Table13" displayName="Table13" ref="A1:F40" totalsRowShown="0">
-  <autoFilter ref="A1:F40" xr:uid="{49FF0015-CF5A-4409-BACE-DDB4A572741A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F1800A77-6274-4EBD-A91A-8D8CA5AD2BBD}" name="Table13" displayName="Table13" ref="A1:F41" totalsRowShown="0">
+  <autoFilter ref="A1:F41" xr:uid="{49FF0015-CF5A-4409-BACE-DDB4A572741A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F40">
     <sortCondition ref="C1:C40"/>
   </sortState>
@@ -2326,10 +2326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867C9CE1-D522-4726-9B57-3B7551A7F9DC}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,33 +2367,25 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>588</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>473575</v>
+        <v>473362</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B5">
-        <v>473362</v>
+        <v>473498</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="B6">
-        <v>473498</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7">
         <v>473501</v>
       </c>
     </row>
@@ -2403,9 +2395,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
     <cfRule type="duplicateValues" dxfId="8" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2416,9 +2405,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D37F582-6F4E-4CA8-BCEC-157E963C8490}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2992,24 +2983,35 @@
         <v>22</v>
       </c>
     </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>588</v>
+      </c>
+      <c r="D41">
+        <v>473575</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A6">
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
     <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A7:A31 A2:A5">
-    <cfRule type="duplicateValues" dxfId="4" priority="231"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="232"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E31 E2:E5">
-    <cfRule type="duplicateValues" dxfId="3" priority="233"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="234"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C40">
-    <cfRule type="duplicateValues" dxfId="2" priority="240"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="241"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C40">
-    <cfRule type="duplicateValues" dxfId="1" priority="243"/>
+  <conditionalFormatting sqref="C2:C41">
+    <cfRule type="duplicateValues" dxfId="2" priority="244"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>